<commit_message>
Added the updated LipSync Manual, LipSync Macro User Guide, LipSync Macro Startup Guide, and LipSync Macro BOM File.
</commit_message>
<xml_diff>
--- a/LipSync_Macro_BOM.xlsx
+++ b/LipSync_Macro_BOM.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristina Mok\Dropbox\NSS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C27C0F-6C04-4AD4-8AFB-C022067D4D28}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1770" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15588" windowHeight="9168"/>
   </bookViews>
   <sheets>
     <sheet name="LipSync_BOM" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="227">
   <si>
     <t>Qty</t>
   </si>
@@ -156,21 +155,9 @@
     <t>http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">1-Position Straight Female Through-Hole Header </t>
-  </si>
-  <si>
-    <t>929974-01-01</t>
-  </si>
-  <si>
     <t>3M</t>
   </si>
   <si>
-    <t>929974-01-01-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">4-Position Straight Female Through-Hole Header  </t>
   </si>
   <si>
@@ -480,18 +467,9 @@
     <t>Screws Phillips Head M3</t>
   </si>
   <si>
-    <t xml:space="preserve">RP809-ND </t>
-  </si>
-  <si>
     <t xml:space="preserve">NMS-308 </t>
   </si>
   <si>
-    <t xml:space="preserve">Essentra Components </t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">SJ5003-0-ND </t>
   </si>
   <si>
@@ -552,9 +530,6 @@
     <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/essentra-components/NMS-308/RP809-ND</t>
-  </si>
-  <si>
     <t>http://www.digikey.ca/product-detail/en/interlink-electronics/30-49649/1027-1000-ND</t>
   </si>
   <si>
@@ -591,9 +566,6 @@
     <t>http://www.digikey.com/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/3m/929974-01-01/929974-01-01-ND</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/keystone-electronics/25503/36-25503-ND/</t>
   </si>
   <si>
@@ -723,31 +695,22 @@
     <t>https://www.leespring.com/compression-springs?search=LC016C03S</t>
   </si>
   <si>
-    <t>Component name (August 12, 2019)</t>
-  </si>
-  <si>
-    <t>SparkFun Bluetooth Mate Silver</t>
-  </si>
-  <si>
-    <t>WRL-12576</t>
-  </si>
-  <si>
-    <t>SparkFun Electronics</t>
-  </si>
-  <si>
-    <t>1568-1265-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND/5762415</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/sparkfun-electronics/WRL-12576/1568-1265-ND/5762415</t>
+    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/97790803211/10056393</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/97790803211/10056393</t>
+  </si>
+  <si>
+    <t>732-13710-ND</t>
+  </si>
+  <si>
+    <t>Component name (July 10, 2020)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1234,13 +1197,16 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1597,10 +1563,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -1624,10 +1590,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1636,7 +1602,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1666,10 +1632,10 @@
         <v>4</v>
       </c>
       <c r="P1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="Q1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -1703,10 +1669,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1715,22 +1681,22 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -1738,7 +1704,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1750,7 +1716,7 @@
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G4" t="s">
         <v>21</v>
@@ -1762,7 +1728,7 @@
         <v>24</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -1770,31 +1736,31 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -1802,31 +1768,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -1834,7 +1800,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -1846,7 +1812,7 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
@@ -1855,13 +1821,13 @@
         <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1869,34 +1835,34 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1904,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -1916,7 +1882,7 @@
         <v>29</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="G9" t="s">
         <v>35</v>
@@ -1925,13 +1891,13 @@
         <v>36</v>
       </c>
       <c r="I9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1939,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -1951,22 +1917,22 @@
         <v>29</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="G10" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -1974,31 +1940,31 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G11" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2006,31 +1972,31 @@
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2038,31 +2004,31 @@
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -2070,31 +2036,31 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" t="s">
-        <v>51</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="Q14" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -2102,31 +2068,31 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2134,31 +2100,31 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2166,31 +2132,31 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -2198,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -2210,7 +2176,7 @@
         <v>40</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G18" t="s">
         <v>39</v>
@@ -2222,7 +2188,7 @@
         <v>42</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
@@ -2230,31 +2196,31 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19" t="s">
+        <v>122</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D19" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" t="s">
-        <v>124</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G19" t="s">
-        <v>125</v>
-      </c>
-      <c r="H19" t="s">
-        <v>126</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="Q19" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -2262,31 +2228,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G20" t="s">
+        <v>210</v>
+      </c>
+      <c r="J20" t="s">
+        <v>210</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G20" t="s">
-        <v>219</v>
-      </c>
-      <c r="J20" t="s">
-        <v>219</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="Q20" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -2294,31 +2260,31 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -2326,31 +2292,31 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -2358,31 +2324,31 @@
         <v>4</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G23" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" t="s">
+        <v>69</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q23" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G23" t="s">
-        <v>71</v>
-      </c>
-      <c r="H23" t="s">
-        <v>73</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2390,31 +2356,31 @@
         <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
+      </c>
+      <c r="E24" t="s">
+        <v>22</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>152</v>
+        <v>204</v>
+      </c>
+      <c r="G24" s="5">
+        <v>97790803211</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>151</v>
+        <v>225</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>154</v>
+        <v>223</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -2422,31 +2388,31 @@
         <v>6</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
@@ -2454,34 +2420,34 @@
         <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G26" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G26" t="s">
-        <v>84</v>
-      </c>
       <c r="H26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I26" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -2489,34 +2455,34 @@
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" t="s">
+        <v>190</v>
+      </c>
+      <c r="P27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D27" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" t="s">
-        <v>80</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G27" t="s">
-        <v>79</v>
-      </c>
-      <c r="H27" t="s">
-        <v>81</v>
-      </c>
-      <c r="I27" t="s">
-        <v>199</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="Q27" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -2524,31 +2490,31 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E28" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2556,34 +2522,34 @@
         <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="I29" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -2591,31 +2557,31 @@
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D30" s="4">
         <v>4708</v>
       </c>
       <c r="E30" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="G30" s="4">
         <v>4708</v>
       </c>
       <c r="H30" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -2623,31 +2589,31 @@
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E31" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="G31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -2655,34 +2621,34 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G32" t="s">
+        <v>94</v>
+      </c>
+      <c r="H32" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" t="s">
+        <v>192</v>
+      </c>
+      <c r="P32" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D32" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G32" t="s">
-        <v>98</v>
-      </c>
-      <c r="H32" t="s">
-        <v>100</v>
-      </c>
-      <c r="I32" t="s">
-        <v>201</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="Q32" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
@@ -2690,31 +2656,31 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G33" t="s">
+        <v>99</v>
+      </c>
+      <c r="N33" t="s">
+        <v>101</v>
+      </c>
+      <c r="P33" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D33" t="s">
-        <v>103</v>
-      </c>
-      <c r="E33" t="s">
-        <v>104</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G33" t="s">
-        <v>103</v>
-      </c>
-      <c r="N33" t="s">
-        <v>105</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="Q33" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
@@ -2722,31 +2688,31 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E34" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G34" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O34" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
@@ -2754,37 +2720,37 @@
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G35" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O35" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="R35" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="S35" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2792,31 +2758,31 @@
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E36" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F36" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G36" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="O36" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
@@ -2824,31 +2790,31 @@
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C37" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
+        <v>200</v>
+      </c>
+      <c r="E37" t="s">
+        <v>199</v>
+      </c>
+      <c r="F37" t="s">
         <v>209</v>
       </c>
-      <c r="E37" t="s">
-        <v>208</v>
-      </c>
-      <c r="F37" t="s">
-        <v>218</v>
-      </c>
       <c r="G37" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I37" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="P37" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="Q37" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
@@ -2856,168 +2822,99 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D38" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E38" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F38" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="G38" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="O38" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>158</v>
-      </c>
-      <c r="C39" t="s">
-        <v>233</v>
-      </c>
-      <c r="D39" t="s">
-        <v>234</v>
-      </c>
-      <c r="E39" t="s">
-        <v>235</v>
-      </c>
-      <c r="F39" t="s">
-        <v>210</v>
-      </c>
-      <c r="G39" t="s">
-        <v>234</v>
-      </c>
-      <c r="H39" t="s">
-        <v>236</v>
-      </c>
-      <c r="P39" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>158</v>
-      </c>
-      <c r="C40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" t="s">
-        <v>45</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G40" t="s">
-        <v>44</v>
-      </c>
-      <c r="H40" t="s">
-        <v>46</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="P7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="P6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="P19" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="P10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="P8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="P9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="P18" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="P40" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="P14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="P12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="P11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="P15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="P16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="P17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="P21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="P22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="P23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="P24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="P27" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="P26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="P28" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="P30" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="P31" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="P32" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="P33" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="P38" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="P3" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="P4" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="P13" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="Q3" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="Q4" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="Q5" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="Q6" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="Q7" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="Q8" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="Q9" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="Q10" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="Q11" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="Q12" r:id="rId40" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="Q13" r:id="rId41" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="Q14" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="Q15" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="Q16" r:id="rId44" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="Q17" r:id="rId45" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="Q18" r:id="rId46" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="Q19" r:id="rId47" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="Q40" r:id="rId48" display="http://www.digikey.ca/product-detail/en/3m/929974-01-01/929974-01-01-ND" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="Q21" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="Q22" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="Q23" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="Q24" r:id="rId52" display="https://www.digikey.ca/product-detail/en/essentra-components/NMS-308/RP809-ND" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="Q26" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="Q27" r:id="rId54" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="Q28" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="Q29" r:id="rId56" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="Q30" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="Q31" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="Q32" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="Q34" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="Q35" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="Q36" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="Q38" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="P34" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="P35" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="Q33" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="P25" r:id="rId67" xr:uid="{4CCDA3FE-08D0-46DF-9B30-73A601C4D5A0}"/>
-    <hyperlink ref="Q25" r:id="rId68" xr:uid="{4DAFF11F-FB4D-4481-B87D-4D729F143D51}"/>
-    <hyperlink ref="Q39" r:id="rId69" xr:uid="{E2C07D5B-A2F3-42F7-987F-7A51DAB010DE}"/>
+    <hyperlink ref="P5" r:id="rId1"/>
+    <hyperlink ref="P7" r:id="rId2"/>
+    <hyperlink ref="P6" r:id="rId3"/>
+    <hyperlink ref="P19" r:id="rId4"/>
+    <hyperlink ref="P10" r:id="rId5"/>
+    <hyperlink ref="P8" r:id="rId6"/>
+    <hyperlink ref="P9" r:id="rId7"/>
+    <hyperlink ref="P18" r:id="rId8"/>
+    <hyperlink ref="P14" r:id="rId9"/>
+    <hyperlink ref="P12" r:id="rId10"/>
+    <hyperlink ref="P11" r:id="rId11"/>
+    <hyperlink ref="P15" r:id="rId12"/>
+    <hyperlink ref="P16" r:id="rId13"/>
+    <hyperlink ref="P17" r:id="rId14"/>
+    <hyperlink ref="P21" r:id="rId15"/>
+    <hyperlink ref="P22" r:id="rId16"/>
+    <hyperlink ref="P23" r:id="rId17"/>
+    <hyperlink ref="P27" r:id="rId18"/>
+    <hyperlink ref="P26" r:id="rId19"/>
+    <hyperlink ref="P28" r:id="rId20"/>
+    <hyperlink ref="P30" r:id="rId21"/>
+    <hyperlink ref="P31" r:id="rId22"/>
+    <hyperlink ref="P32" r:id="rId23"/>
+    <hyperlink ref="P33" r:id="rId24"/>
+    <hyperlink ref="P38" r:id="rId25"/>
+    <hyperlink ref="P3" r:id="rId26"/>
+    <hyperlink ref="P4" r:id="rId27"/>
+    <hyperlink ref="P13" r:id="rId28"/>
+    <hyperlink ref="Q3" r:id="rId29"/>
+    <hyperlink ref="Q4" r:id="rId30"/>
+    <hyperlink ref="Q5" r:id="rId31"/>
+    <hyperlink ref="Q6" r:id="rId32"/>
+    <hyperlink ref="Q7" r:id="rId33"/>
+    <hyperlink ref="Q8" r:id="rId34"/>
+    <hyperlink ref="Q9" r:id="rId35"/>
+    <hyperlink ref="Q10" r:id="rId36"/>
+    <hyperlink ref="Q11" r:id="rId37"/>
+    <hyperlink ref="Q12" r:id="rId38" display="https://www.digikey.ca/product-detail/en/molex-connector-corporation/22-05-2031/WM4101-ND/"/>
+    <hyperlink ref="Q13" r:id="rId39" display="https://www.digikey.ca/product-detail/en/preci-dip/801-87-003-10-001101/1212-1180-ND"/>
+    <hyperlink ref="Q14" r:id="rId40"/>
+    <hyperlink ref="Q15" r:id="rId41"/>
+    <hyperlink ref="Q16" r:id="rId42" display="https://www.digikey.ca/product-detail/en/everlight-electronics-co-ltd/MV5437/1080-1109-ND/2675600"/>
+    <hyperlink ref="Q17" r:id="rId43" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/SPC02SYAN/S9002-ND"/>
+    <hyperlink ref="Q18" r:id="rId44" display="http://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/2N3906TFR/2N3906D26ZCT-ND"/>
+    <hyperlink ref="Q19" r:id="rId45" display="https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC061LFBN-RC/S7039-ND"/>
+    <hyperlink ref="Q21" r:id="rId46"/>
+    <hyperlink ref="Q22" r:id="rId47"/>
+    <hyperlink ref="Q23" r:id="rId48"/>
+    <hyperlink ref="Q26" r:id="rId49"/>
+    <hyperlink ref="Q27" r:id="rId50" display="http://www.digikey.ca/product-detail/en/keystone-electronics/25503/36-25503-ND/"/>
+    <hyperlink ref="Q28" r:id="rId51"/>
+    <hyperlink ref="Q29" r:id="rId52" display="https://www.digikey.ca/product-detail/en/3m/SJ-5003-(BLACK)/SJ5003-0-ND/102573"/>
+    <hyperlink ref="Q30" r:id="rId53"/>
+    <hyperlink ref="Q31" r:id="rId54"/>
+    <hyperlink ref="Q32" r:id="rId55"/>
+    <hyperlink ref="Q34" r:id="rId56"/>
+    <hyperlink ref="Q35" r:id="rId57"/>
+    <hyperlink ref="Q36" r:id="rId58"/>
+    <hyperlink ref="Q38" r:id="rId59"/>
+    <hyperlink ref="P34" r:id="rId60"/>
+    <hyperlink ref="P35" r:id="rId61"/>
+    <hyperlink ref="Q33" r:id="rId62"/>
+    <hyperlink ref="P25" r:id="rId63"/>
+    <hyperlink ref="Q25" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>